<commit_message>
every parent at max iop
</commit_message>
<xml_diff>
--- a/ea_order.xlsx
+++ b/ea_order.xlsx
@@ -2497,6 +2497,9 @@
     <t>V43_C27</t>
   </si>
   <si>
+    <t>V34_C1</t>
+  </si>
+  <si>
     <t>V44_C8</t>
   </si>
   <si>
@@ -2504,9 +2507,6 @@
   </si>
   <si>
     <t>V31_C10</t>
-  </si>
-  <si>
-    <t>V34_C1</t>
   </si>
   <si>
     <t>V39_C2</t>
@@ -5029,13 +5029,13 @@
         <v>211.52</v>
       </c>
       <c r="G34">
-        <v>215.82</v>
+        <v>265</v>
       </c>
       <c r="H34">
         <v>125</v>
       </c>
       <c r="I34">
-        <v>49.18000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -18344,28 +18344,28 @@
         <v>517</v>
       </c>
       <c r="B519" t="s">
-        <v>209</v>
+        <v>246</v>
       </c>
       <c r="C519" t="s">
         <v>827</v>
       </c>
       <c r="D519">
-        <v>0.00713</v>
+        <v>0.00749</v>
       </c>
       <c r="E519">
-        <v>127.85</v>
+        <v>31.19</v>
       </c>
       <c r="F519">
-        <v>185.77</v>
+        <v>186.11</v>
       </c>
       <c r="G519">
-        <v>185.94</v>
+        <v>186</v>
       </c>
       <c r="H519">
         <v>96.8</v>
       </c>
       <c r="I519">
-        <v>79.06</v>
+        <v>79</v>
       </c>
     </row>
     <row r="520" spans="1:9">
@@ -18373,28 +18373,28 @@
         <v>518</v>
       </c>
       <c r="B520" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C520" t="s">
         <v>828</v>
       </c>
       <c r="D520">
-        <v>0.00721</v>
+        <v>0.00713</v>
       </c>
       <c r="E520">
-        <v>210.55</v>
+        <v>127.85</v>
       </c>
       <c r="F520">
-        <v>180.17</v>
+        <v>185.77</v>
       </c>
       <c r="G520">
-        <v>185.93</v>
+        <v>185.94</v>
       </c>
       <c r="H520">
         <v>96.8</v>
       </c>
       <c r="I520">
-        <v>79.06999999999999</v>
+        <v>79.06</v>
       </c>
     </row>
     <row r="521" spans="1:9">
@@ -18402,28 +18402,28 @@
         <v>519</v>
       </c>
       <c r="B521" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="C521" t="s">
         <v>829</v>
       </c>
       <c r="D521">
-        <v>0.0083</v>
+        <v>0.00721</v>
       </c>
       <c r="E521">
-        <v>97.45</v>
+        <v>210.55</v>
       </c>
       <c r="F521">
-        <v>185.12</v>
+        <v>180.17</v>
       </c>
       <c r="G521">
-        <v>185.91</v>
+        <v>185.93</v>
       </c>
       <c r="H521">
         <v>96.8</v>
       </c>
       <c r="I521">
-        <v>79.09</v>
+        <v>79.06999999999999</v>
       </c>
     </row>
     <row r="522" spans="1:9">
@@ -18431,28 +18431,28 @@
         <v>520</v>
       </c>
       <c r="B522" t="s">
-        <v>246</v>
+        <v>183</v>
       </c>
       <c r="C522" t="s">
         <v>830</v>
       </c>
       <c r="D522">
-        <v>0.00749</v>
+        <v>0.0083</v>
       </c>
       <c r="E522">
-        <v>31.19</v>
+        <v>97.45</v>
       </c>
       <c r="F522">
-        <v>186.11</v>
+        <v>185.12</v>
       </c>
       <c r="G522">
-        <v>185.86</v>
+        <v>185.91</v>
       </c>
       <c r="H522">
         <v>96.8</v>
       </c>
       <c r="I522">
-        <v>79.13999999999999</v>
+        <v>79.09</v>
       </c>
     </row>
     <row r="523" spans="1:9">

</xml_diff>